<commit_message>
Updates from testing tabtools
</commit_message>
<xml_diff>
--- a/_testing/output/tablex_test1.xlsx
+++ b/_testing/output/tablex_test1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="112" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="22">
   <si>
     <t>Test 1: Frequency Table</t>
   </si>
@@ -85,10 +85,797 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="375">
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+  <fonts count="562">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1673,7 +2460,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="253">
+  <borders count="379">
     <border>
       <left/>
       <right/>
@@ -3397,11 +4184,869 @@
       <bottom style="thin"/>
       <diagonal style="none"/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="379">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -4384,6 +6029,498 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="374" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="254" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="255" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="256" xfId="0"/>
+    <xf numFmtId="0" fontId="375" fillId="0" borderId="257" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="376" fillId="0" borderId="258" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="377" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="378" fillId="0" borderId="260" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="379" fillId="0" borderId="261" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="380" fillId="0" borderId="262" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="381" fillId="0" borderId="263" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="382" fillId="0" borderId="264" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="383" fillId="0" borderId="265" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="384" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="385" fillId="0" borderId="267" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="386" fillId="0" borderId="268" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="387" fillId="0" borderId="269" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="388" fillId="0" borderId="270" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="389" fillId="0" borderId="271" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="390" fillId="0" borderId="272" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="392" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="394" fillId="0" borderId="274" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="396" fillId="0" borderId="275" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="398" fillId="0" borderId="276" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="400" fillId="0" borderId="277" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="402" fillId="0" borderId="278" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="404" fillId="0" borderId="279" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="406" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="408" fillId="0" borderId="281" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="410" fillId="0" borderId="282" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="412" fillId="0" borderId="283" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="414" fillId="0" borderId="284" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="416" fillId="0" borderId="285" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="418" fillId="0" borderId="286" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="420" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="422" fillId="0" borderId="288" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="423" fillId="0" borderId="289" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="424" fillId="0" borderId="290" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="425" fillId="0" borderId="291" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="426" fillId="0" borderId="292" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="427" fillId="0" borderId="293" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="428" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="429" fillId="0" borderId="295" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="430" fillId="0" borderId="296" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="432" fillId="0" borderId="297" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="434" fillId="0" borderId="298" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="436" fillId="0" borderId="299" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="438" fillId="0" borderId="300" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="440" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="442" fillId="0" borderId="302" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="444" fillId="0" borderId="303" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="446" fillId="0" borderId="304" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="448" fillId="0" borderId="305" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="450" fillId="0" borderId="306" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="452" fillId="0" borderId="307" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="454" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="456" fillId="0" borderId="309" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="458" fillId="0" borderId="310" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="459" fillId="0" borderId="311" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="460" fillId="0" borderId="312" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="461" fillId="0" borderId="313" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="462" fillId="0" borderId="314" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="463" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="464" fillId="0" borderId="316" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="465" fillId="0" borderId="317" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="466" fillId="0" borderId="318" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="467" fillId="0" borderId="319" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="468" fillId="0" borderId="320" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="469" fillId="0" borderId="321" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="470" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="471" fillId="0" borderId="323" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="472" fillId="0" borderId="324" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="473" fillId="0" borderId="325" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="474" fillId="0" borderId="326" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="475" fillId="0" borderId="327" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="476" fillId="0" borderId="328" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="477" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="478" fillId="0" borderId="330" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="479" fillId="0" borderId="331" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="480" fillId="0" borderId="332" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="481" fillId="0" borderId="333" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="482" fillId="0" borderId="334" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="483" fillId="0" borderId="335" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="484" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="485" fillId="0" borderId="337" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="486" fillId="0" borderId="338" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="487" fillId="0" borderId="339" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="488" fillId="0" borderId="340" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="489" fillId="0" borderId="341" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="490" fillId="0" borderId="342" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="491" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="493" fillId="0" borderId="344" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="495" fillId="0" borderId="345" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="497" fillId="0" borderId="346" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="499" fillId="0" borderId="347" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="501" fillId="0" borderId="348" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="503" fillId="0" borderId="349" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="505" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="507" fillId="0" borderId="351" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="509" fillId="0" borderId="352" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="511" fillId="0" borderId="353" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="513" fillId="0" borderId="354" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="515" fillId="0" borderId="355" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="517" fillId="0" borderId="356" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="519" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="521" fillId="0" borderId="358" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="523" fillId="0" borderId="359" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="525" fillId="0" borderId="360" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="527" fillId="0" borderId="361" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="529" fillId="0" borderId="362" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="531" fillId="0" borderId="363" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="533" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="535" fillId="0" borderId="365" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="537" fillId="0" borderId="366" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="539" fillId="0" borderId="367" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="541" fillId="0" borderId="368" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="543" fillId="0" borderId="369" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="545" fillId="0" borderId="370" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="547" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="549" fillId="0" borderId="372" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="551" fillId="0" borderId="373" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="553" fillId="0" borderId="374" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="555" fillId="0" borderId="375" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="557" fillId="0" borderId="376" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="559" fillId="0" borderId="377" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="561" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4402,190 +6539,190 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="128" customWidth="true"/>
-    <col min="2" max="2" width="12.7109375" style="129" customWidth="true"/>
-    <col min="3" max="8" width="16.7109375" style="130" customWidth="true"/>
+    <col min="1" max="1" width="2.7109375" style="254" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" style="255" customWidth="true"/>
+    <col min="3" max="8" width="16.7109375" style="256" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="127" customFormat="true" ht="30" customHeight="true">
-      <c r="A1" s="163" t="s">
+    <row r="1" s="253" customFormat="true" ht="30" customHeight="true">
+      <c r="A1" s="289" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163" t="s">
+      <c r="B1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="163" t="s">
+      <c r="C1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="163" t="s">
+      <c r="D1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="163" t="s">
+      <c r="E1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="163" t="s">
+      <c r="F1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="163" t="s">
+      <c r="G1" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="163" t="s">
+      <c r="H1" s="289" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="325" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="193" t="s">
+      <c r="C2" s="319" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="194" t="s">
+      <c r="D2" s="320" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="195" t="s">
+      <c r="E2" s="321" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="196" t="s">
+      <c r="F2" s="322" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="197" t="s">
+      <c r="G2" s="323" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="205" t="s">
+      <c r="H2" s="331" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="218" t="s">
+      <c r="B3" s="344" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="219" t="s">
+      <c r="C3" s="345" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="220" t="s">
+      <c r="D3" s="346" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="221" t="s">
+      <c r="E3" s="347" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="222" t="s">
+      <c r="F3" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="223" t="s">
+      <c r="G3" s="349" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="224" t="s">
+      <c r="H3" s="350" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="351" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="226" t="s">
+      <c r="C4" s="352" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="227" t="s">
+      <c r="D4" s="353" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="228" t="s">
+      <c r="E4" s="354" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="229" t="s">
+      <c r="F4" s="355" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="230" t="s">
+      <c r="G4" s="356" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="231" t="s">
+      <c r="H4" s="357" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="232" t="s">
+      <c r="B5" s="358" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="233" t="s">
+      <c r="C5" s="359" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="234" t="s">
+      <c r="D5" s="360" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="235" t="s">
+      <c r="E5" s="361" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="236" t="s">
+      <c r="F5" s="362" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="237" t="s">
+      <c r="G5" s="363" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="238" t="s">
+      <c r="H5" s="364" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="239" t="s">
+      <c r="B6" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="240" t="s">
+      <c r="C6" s="366" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="241" t="s">
+      <c r="D6" s="367" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="242" t="s">
+      <c r="E6" s="368" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="243" t="s">
+      <c r="F6" s="369" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="244" t="s">
+      <c r="G6" s="370" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="245" t="s">
+      <c r="H6" s="371" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="246" t="s">
+      <c r="B7" s="372" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="247" t="s">
+      <c r="C7" s="373" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="248" t="s">
+      <c r="D7" s="374" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="249" t="s">
+      <c r="E7" s="375" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="250" t="s">
+      <c r="F7" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="251" t="s">
+      <c r="G7" s="377" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="252" t="s">
+      <c r="H7" s="378" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>